<commit_message>
Finalisation des scénarios de testes
</commit_message>
<xml_diff>
--- a/Documentation/Scénario test.xlsx
+++ b/Documentation/Scénario test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\BatailleNavale\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DA7E50-BA87-46A3-A141-73E9E7BCBB32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659D9B9D-19A2-4830-B5D5-387C39A9E8B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Scénario</t>
   </si>
@@ -43,6 +43,33 @@
   </si>
   <si>
     <t>Lancement du programme</t>
+  </si>
+  <si>
+    <t>Le joueur s'authentifie</t>
+  </si>
+  <si>
+    <t>le joueur entre des coordonnées invalide</t>
+  </si>
+  <si>
+    <t>le joueur entre des coordonnées valide</t>
+  </si>
+  <si>
+    <t>le joueur touche un bateau</t>
+  </si>
+  <si>
+    <t>le joueur coule un bateau</t>
+  </si>
+  <si>
+    <t>le joueur à gagner</t>
+  </si>
+  <si>
+    <t>enregistrement du score</t>
+  </si>
+  <si>
+    <t>quitter le programme</t>
+  </si>
+  <si>
+    <t>affichage des scores</t>
   </si>
 </sst>
 </file>
@@ -66,7 +93,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -74,11 +101,146 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -88,6 +250,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -369,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:G18"/>
+  <dimension ref="C3:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -382,96 +571,115 @@
     <col min="8" max="8" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:7" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="2" t="s">
+    <row r="3" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="3:7" ht="54.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C5" s="2" t="s">
+    <row r="5" spans="3:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="3:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="2"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="3:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="2"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="3:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="2"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="3:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="2"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="3:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="2"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="3:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="2"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="3:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="2"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="2"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C14" s="2"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="3:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="3:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="3:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="3:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="3:7" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="3:7" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="3:7" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="3:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="3:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
+    </row>
+    <row r="15" spans="3:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C15" s="2"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -501,5 +709,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>